<commit_message>
Archive 11/04 files. Update commonness index calculations. Update readme file. Rename R and .do files and clean up master files.
</commit_message>
<xml_diff>
--- a/output/20221104/tables/hh_regs_no_effort/betas.xlsx
+++ b/output/20221104/tables/hh_regs_no_effort/betas.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erb32/github/cambodia_biodiversity2/output/20221104/tables/hh_regs_no_effort/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEBDC84-8F24-8B40-B901-797A25D5EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Species count models" sheetId="1" r:id="rId2"/>
+    <sheet name="Species count models" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
   <si>
     <t>Outcome</t>
   </si>
@@ -72,8 +92,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -95,27 +118,344 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -144,7 +484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -154,11 +494,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.34650340676307678</v>
       </c>
       <c r="E2" s="1">
-        <v>0.093618355691432953</v>
+        <v>9.3618355691432953E-2</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -173,7 +513,7 @@
         <v>0.53374010324478149</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -183,11 +523,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>0.3501109778881073</v>
       </c>
       <c r="E3" s="1">
-        <v>0.091486096382141113</v>
+        <v>9.1486096382141113E-2</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -202,7 +542,7 @@
         <v>0.53308320045471191</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -212,11 +552,11 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>0.37285584211349487</v>
       </c>
       <c r="E4" s="1">
-        <v>0.085471294820308685</v>
+        <v>8.5471294820308685E-2</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -231,7 +571,7 @@
         <v>0.54379844665527344</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -241,11 +581,11 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0.89913344383239746</v>
       </c>
       <c r="E5" s="1">
-        <v>0.020791295915842056</v>
+        <v>2.0791295915842056E-2</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -260,7 +600,7 @@
         <v>0.94071602821350098</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -270,11 +610,11 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0.89727693796157837</v>
       </c>
       <c r="E6" s="1">
-        <v>0.01982947438955307</v>
+        <v>1.982947438955307E-2</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
@@ -289,7 +629,7 @@
         <v>0.9369359016418457</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -299,11 +639,11 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0.89582264423370361</v>
       </c>
       <c r="E7" s="1">
-        <v>0.019301192834973335</v>
+        <v>1.9301192834973335E-2</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -318,7 +658,7 @@
         <v>0.93442505598068237</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -328,11 +668,11 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>0.2708798348903656</v>
       </c>
       <c r="E8" s="1">
-        <v>0.039570342749357224</v>
+        <v>3.9570342749357224E-2</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -347,7 +687,7 @@
         <v>0.35002052783966064</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -357,11 +697,11 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>0.27627730369567871</v>
       </c>
       <c r="E9" s="1">
-        <v>0.036794524639844894</v>
+        <v>3.6794524639844894E-2</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -376,7 +716,7 @@
         <v>0.3498663604259491</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -386,11 +726,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>0.28031918406486511</v>
       </c>
       <c r="E10" s="1">
-        <v>0.038133770227432251</v>
+        <v>3.8133770227432251E-2</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -405,7 +745,7 @@
         <v>0.35658672451972961</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -415,11 +755,11 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0.29589375853538513</v>
       </c>
       <c r="E11" s="1">
-        <v>0.081302262842655182</v>
+        <v>8.1302262842655182E-2</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -434,7 +774,7 @@
         <v>0.45849829912185669</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -444,11 +784,11 @@
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>0.30266293883323669</v>
       </c>
       <c r="E12" s="1">
-        <v>0.078538224101066589</v>
+        <v>7.8538224101066589E-2</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -463,7 +803,7 @@
         <v>0.45973938703536987</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -473,11 +813,11 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>0.32400384545326233</v>
       </c>
       <c r="E13" s="1">
-        <v>0.071458756923675537</v>
+        <v>7.1458756923675537E-2</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -492,7 +832,7 @@
         <v>0.4669213593006134</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -502,11 +842,11 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1">
-        <v>0.063580483198165894</v>
+      <c r="D14" s="2">
+        <v>6.3580483198165894E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>0.035771388560533524</v>
+        <v>3.5771388560533524E-2</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -515,13 +855,13 @@
         <v>15</v>
       </c>
       <c r="H14" s="1">
-        <v>-0.0079622939229011536</v>
+        <v>-7.9622939229011536E-3</v>
       </c>
       <c r="I14" s="1">
         <v>0.13512325286865234</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -531,11 +871,11 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1">
-        <v>0.053387299180030823</v>
+      <c r="D15" s="2">
+        <v>5.3387299180030823E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>0.035245683044195175</v>
+        <v>3.5245683044195175E-2</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -544,13 +884,13 @@
         <v>15</v>
       </c>
       <c r="H15" s="1">
-        <v>-0.017104066908359528</v>
+        <v>-1.7104066908359528E-2</v>
       </c>
       <c r="I15" s="1">
         <v>0.12387866526842117</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -560,11 +900,11 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.0559505894780159</v>
+      <c r="D16" s="2">
+        <v>5.59505894780159E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>0.034688640385866165</v>
+        <v>3.4688640385866165E-2</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -573,12 +913,13 @@
         <v>15</v>
       </c>
       <c r="H16" s="1">
-        <v>-0.013426691293716431</v>
+        <v>-1.3426691293716431E-2</v>
       </c>
       <c r="I16" s="1">
         <v>0.12532787024974823</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>